<commit_message>
Auto-committed on 2021/12/27 週一
Former-commit-id: bb5a542f93cfaa80ebb8d4846589d7d44b5d3246
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/FacShareLimit.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/FacShareLimit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L2-業務作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35AD843-8EE6-4156-A4DD-52011F2897E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6B5CC7-ECF1-4584-86F6-ECC1E6488E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,7 +828,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -842,7 +842,7 @@
     <col min="8" max="16384" width="21.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>28</v>
       </c>
       <c r="E13" s="11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="21"/>

</xml_diff>